<commit_message>
Update: Add atmega328 cost
</commit_message>
<xml_diff>
--- a/Documents/Cost.xlsx
+++ b/Documents/Cost.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2727A6E0-31F8-497D-8F76-4D6499729FE2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB045092-1BA8-4C69-B98D-689F4BBA0C84}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>No.</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>Buy second hand from Thong</t>
+  </si>
+  <si>
+    <t>ATmega328p-AU</t>
+  </si>
+  <si>
+    <t>Thegioiic</t>
   </si>
 </sst>
 </file>
@@ -433,7 +439,7 @@
   <dimension ref="A1:G156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -526,11 +532,21 @@
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="B6" s="5">
+        <v>43273</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="6">
+        <v>55000</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update: Logs, Cost for buying components
</commit_message>
<xml_diff>
--- a/Documents/Cost.xlsx
+++ b/Documents/Cost.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB045092-1BA8-4C69-B98D-689F4BBA0C84}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F13724-B6B0-4D61-95C1-ADA43732DC03}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>No.</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>Thegioiic</t>
+  </si>
+  <si>
+    <t>Bill number 32271</t>
+  </si>
+  <si>
+    <t>ESP8266-V12 + AMS1117 3v3 + Resistor 330Ohm 0805 + Button + Cap 10uF 0805</t>
   </si>
 </sst>
 </file>
@@ -135,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -154,6 +160,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -439,21 +448,21 @@
   <dimension ref="A1:G156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="28.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="57.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="35.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="28.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="57.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
@@ -461,7 +470,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -484,7 +493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -505,7 +514,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -528,7 +537,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -549,18 +558,30 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="5">
+        <v>43285</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="8">
+        <v>67500</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -571,7 +592,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -582,7 +603,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -593,7 +614,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -604,7 +625,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -615,7 +636,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -626,7 +647,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -637,7 +658,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -648,7 +669,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -659,7 +680,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -670,7 +691,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -681,7 +702,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -692,7 +713,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -703,412 +724,412 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D32" s="7"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="7"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="7"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="7"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="7"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="7"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="7"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="7"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="7"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="7"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="7"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="7"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="7"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="7"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="7"/>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" s="7"/>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" s="7"/>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" s="7"/>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" s="7"/>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D64" s="7"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="7"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="7"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="7"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="7"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="7"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="7"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="7"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73" s="7"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="7"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75" s="7"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="7"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D78" s="7"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D79" s="7"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="7"/>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="7"/>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D82" s="7"/>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="7"/>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D84" s="7"/>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85" s="7"/>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D86" s="7"/>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D87" s="7"/>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D88" s="7"/>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D89" s="7"/>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D90" s="7"/>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D91" s="7"/>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D92" s="7"/>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D93" s="7"/>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D94" s="7"/>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D95" s="7"/>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D96" s="7"/>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D97" s="7"/>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D98" s="7"/>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D99" s="7"/>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D100" s="7"/>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D101" s="7"/>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D102" s="7"/>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D103" s="7"/>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D104" s="7"/>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D105" s="7"/>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D106" s="7"/>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D107" s="7"/>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D108" s="7"/>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D109" s="7"/>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D110" s="7"/>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D111" s="7"/>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D112" s="7"/>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D113" s="7"/>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D114" s="7"/>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D115" s="7"/>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D116" s="7"/>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D117" s="7"/>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D118" s="7"/>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D119" s="7"/>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D120" s="7"/>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D121" s="7"/>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D122" s="7"/>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D123" s="7"/>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D124" s="7"/>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D125" s="7"/>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D126" s="7"/>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D127" s="7"/>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D128" s="7"/>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D129" s="7"/>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D130" s="7"/>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D131" s="7"/>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D132" s="7"/>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D133" s="7"/>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D134" s="7"/>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D135" s="7"/>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D136" s="7"/>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D137" s="7"/>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D138" s="7"/>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D139" s="7"/>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D140" s="7"/>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D141" s="7"/>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D142" s="7"/>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D143" s="7"/>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D144" s="7"/>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D145" s="7"/>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D146" s="7"/>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D147" s="7"/>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D148" s="7"/>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D149" s="7"/>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D150" s="7"/>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D151" s="7"/>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D152" s="7"/>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D153" s="7"/>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D154" s="7"/>
     </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D155" s="7"/>
     </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D156" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: Add cost of Raspberry Fan
</commit_message>
<xml_diff>
--- a/Documents/Cost.xlsx
+++ b/Documents/Cost.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC21CC3-4949-49D1-B2DE-F51571BF1698}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A3B5FE-9AC6-46FE-94FC-A982FAEB7214}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>No.</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>Bill number 33071</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Fan</t>
+  </si>
+  <si>
+    <t>BanLinhKien.vn</t>
   </si>
 </sst>
 </file>
@@ -638,11 +644,21 @@
       <c r="A10" s="3">
         <v>7</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="B10" s="5">
+        <v>43308</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="6">
+        <v>25000</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update: Update cost for PCBs and components
</commit_message>
<xml_diff>
--- a/Documents/Cost.xlsx
+++ b/Documents/Cost.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A3B5FE-9AC6-46FE-94FC-A982FAEB7214}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE473C7-C4CA-4C72-987D-273BE29B8439}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>No.</t>
   </si>
@@ -92,6 +92,27 @@
   </si>
   <si>
     <t>BanLinhKien.vn</t>
+  </si>
+  <si>
+    <t>RFM95 868MHz</t>
+  </si>
+  <si>
+    <t>TaoBao</t>
+  </si>
+  <si>
+    <t>PCB of LCD_Button_Gateway_Driver &amp; RPi3_LoRaWan_Gateway</t>
+  </si>
+  <si>
+    <t>JLCPCB</t>
+  </si>
+  <si>
+    <t>Bill number 34246</t>
+  </si>
+  <si>
+    <t>Bill number 34506</t>
+  </si>
+  <si>
+    <t>2 x 18650 Battery 3v3 + ATMega328P-AU</t>
   </si>
 </sst>
 </file>
@@ -463,13 +484,13 @@
   <dimension ref="A1:G156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="28.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="57.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
@@ -665,45 +686,87 @@
       <c r="A11" s="3">
         <v>8</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="B11" s="5">
+        <v>43321</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="6">
+        <v>250000</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>9</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="B12" s="5">
+        <v>43321</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="6">
+        <v>350000</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="5">
+        <v>43317</v>
+      </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="D13" s="6">
+        <v>70400</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>11</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="B14" s="5">
+        <v>43321</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="6">
+        <v>293000</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">

</xml_diff>